<commit_message>
Atualiza granularidade da consulta avançada
</commit_message>
<xml_diff>
--- a/espec018_recursos-acordo-judicial-vale/static/cruzamento-dados-monte-sua-pesquisa.xlsx
+++ b/espec018_recursos-acordo-judicial-vale/static/cruzamento-dados-monte-sua-pesquisa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1. CGE\tele-trabalho\GIT\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE314D22-58EE-4C3C-9982-3999467C61C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9CB26F-5062-47FC-A4FD-1590C7925458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F42378E0-2AE5-E64E-B820-AB19A200C1EC}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F42378E0-2AE5-E64E-B820-AB19A200C1EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="171">
   <si>
     <t>Consulta</t>
   </si>
@@ -1027,12 +1027,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA762CE-BD9F-B449-A867-C6DC996C3AFE}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1123,9 @@
       <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
@@ -1176,7 +1178,9 @@
       <c r="H3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1229,7 +1233,9 @@
       <c r="H4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1282,7 +1288,9 @@
       <c r="H5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J5" s="7" t="s">
         <v>7</v>
       </c>
@@ -1331,7 +1339,9 @@
       <c r="H6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J6" s="7" t="s">
         <v>7</v>
       </c>
@@ -1378,7 +1388,9 @@
       <c r="H7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1425,7 +1437,9 @@
       <c r="H8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J8" s="7" t="s">
         <v>7</v>
       </c>
@@ -1472,7 +1486,9 @@
       <c r="H9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="J9" s="7" t="s">
         <v>7</v>
       </c>
@@ -1521,7 +1537,9 @@
       <c r="H10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="13"/>
+      <c r="I10" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="J10" s="13" t="s">
         <v>7</v>
       </c>
@@ -1592,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCAC446-5523-AB48-A89C-19E16A4B024A}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>